<commit_message>
implement sensitivity analysis functionality and create test for multi CPu simulations as a sensitivity analysis case study
</commit_message>
<xml_diff>
--- a/test_data/norfolk_coastal_flooding/cpu_benchmarking_analysis.xlsx
+++ b/test_data/norfolk_coastal_flooding/cpu_benchmarking_analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\src\TRITON_SWMM_toolkit\examples\norfolk_coastal_flooding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\test_data\norfolk_coastal_flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42BDFE29-A7FF-40D9-86AB-AA8970216A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21E1920-E23D-4774-B406-F1D35C768E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="4185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>CPU</t>
   </si>
   <si>
-    <t>MPI_ranks_per_node</t>
-  </si>
-  <si>
     <t>Baseline - 1 CPU</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Multi-CPU - HYB</t>
   </si>
   <si>
-    <t>OpenMP_threads_per_rank</t>
-  </si>
-  <si>
     <t>devices_per_node</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
     <t>device</t>
   </si>
   <si>
-    <t>nodes</t>
-  </si>
-  <si>
     <t>total_MPI_ranks</t>
   </si>
   <si>
@@ -81,6 +72,33 @@
   </si>
   <si>
     <t>selected</t>
+  </si>
+  <si>
+    <t>run_mode</t>
+  </si>
+  <si>
+    <t>serial</t>
+  </si>
+  <si>
+    <t>hybrid</t>
+  </si>
+  <si>
+    <t>openmp</t>
+  </si>
+  <si>
+    <t>mpi</t>
+  </si>
+  <si>
+    <t>n_nodes</t>
+  </si>
+  <si>
+    <t>n_omp_threads</t>
+  </si>
+  <si>
+    <t>n_gpus</t>
+  </si>
+  <si>
+    <t>n_mpi_procs</t>
   </si>
 </sst>
 </file>
@@ -296,7 +314,59 @@
     <cellStyle name="Note" xfId="3" builtinId="10"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -579,13 +649,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -715,24 +785,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11" totalsRowBorderDxfId="10">
-  <autoFilter ref="A1:J5" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J5">
-    <sortCondition ref="J1:J5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}" name="Table1" displayName="Table1" ref="A1:L5" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="A1:L5" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L5">
+    <sortCondition ref="L1:L5"/>
   </sortState>
-  <tableColumns count="10">
-    <tableColumn id="11" xr3:uid="{3DECB62C-AAF2-4EC7-8598-5E8776D4B845}" name="hardware_utilization_strategy" dataDxfId="9" dataCellStyle="Note"/>
-    <tableColumn id="9" xr3:uid="{047B8296-C28F-43DA-A753-CC6445B34CE4}" name="device" dataDxfId="8" dataCellStyle="Note"/>
-    <tableColumn id="2" xr3:uid="{09DC1F4B-B2B0-493A-B83E-1D7D4EA31F4C}" name="nodes" dataDxfId="7" dataCellStyle="Input"/>
-    <tableColumn id="3" xr3:uid="{3A65E5E5-CB8B-4698-A27C-21DF3A95D49A}" name="MPI_ranks_per_node" dataDxfId="6" dataCellStyle="Input"/>
-    <tableColumn id="4" xr3:uid="{D366E835-7967-45B3-94DD-92B04C3126AA}" name="OpenMP_threads_per_rank" dataDxfId="5" dataCellStyle="Input"/>
-    <tableColumn id="5" xr3:uid="{4E090350-4FC8-498D-A3DF-C96FED73C7DB}" name="total_MPI_ranks" dataDxfId="4" dataCellStyle="Output"/>
-    <tableColumn id="6" xr3:uid="{F6B7A6B4-BD4B-4406-BCB7-C3DBCC48FA6B}" name="total_OpenMP_threads" dataDxfId="3" dataCellStyle="Output"/>
-    <tableColumn id="7" xr3:uid="{8B064801-C992-4C19-AF9B-73CC7D0951B1}" name="total_devices" dataDxfId="2" dataCellStyle="Output"/>
-    <tableColumn id="10" xr3:uid="{C813D3D6-6AEA-4168-A5C0-6FD56BB1D36D}" name="devices_per_node" dataDxfId="1" dataCellStyle="Output">
-      <calculatedColumnFormula>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[nodes]]</calculatedColumnFormula>
+  <tableColumns count="12">
+    <tableColumn id="11" xr3:uid="{3DECB62C-AAF2-4EC7-8598-5E8776D4B845}" name="hardware_utilization_strategy" dataDxfId="11" dataCellStyle="Note"/>
+    <tableColumn id="9" xr3:uid="{047B8296-C28F-43DA-A753-CC6445B34CE4}" name="device" dataDxfId="10" dataCellStyle="Note"/>
+    <tableColumn id="8" xr3:uid="{5BB507EE-7025-4DDF-A0F3-C7717F14E194}" name="run_mode" dataDxfId="1" dataCellStyle="Input"/>
+    <tableColumn id="2" xr3:uid="{09DC1F4B-B2B0-493A-B83E-1D7D4EA31F4C}" name="n_nodes" dataDxfId="9" dataCellStyle="Input"/>
+    <tableColumn id="3" xr3:uid="{3A65E5E5-CB8B-4698-A27C-21DF3A95D49A}" name="n_mpi_procs" dataDxfId="8" dataCellStyle="Input"/>
+    <tableColumn id="4" xr3:uid="{D366E835-7967-45B3-94DD-92B04C3126AA}" name="n_omp_threads" dataDxfId="7" dataCellStyle="Input"/>
+    <tableColumn id="12" xr3:uid="{037A1F48-3B4F-4ED2-9C19-A48E0403F1E9}" name="n_gpus" dataDxfId="0" dataCellStyle="Input"/>
+    <tableColumn id="5" xr3:uid="{4E090350-4FC8-498D-A3DF-C96FED73C7DB}" name="total_MPI_ranks" dataDxfId="6" dataCellStyle="Output"/>
+    <tableColumn id="6" xr3:uid="{F6B7A6B4-BD4B-4406-BCB7-C3DBCC48FA6B}" name="total_OpenMP_threads" dataDxfId="5" dataCellStyle="Output"/>
+    <tableColumn id="7" xr3:uid="{8B064801-C992-4C19-AF9B-73CC7D0951B1}" name="total_devices" dataDxfId="4" dataCellStyle="Output"/>
+    <tableColumn id="10" xr3:uid="{C813D3D6-6AEA-4168-A5C0-6FD56BB1D36D}" name="devices_per_node" dataDxfId="3" dataCellStyle="Output">
+      <calculatedColumnFormula>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{819E4573-DBC8-4D9F-8E0A-AED8703E6A04}" name="selected" dataDxfId="0" dataCellStyle="Output"/>
+    <tableColumn id="1" xr3:uid="{819E4573-DBC8-4D9F-8E0A-AED8703E6A04}" name="selected" dataDxfId="2" dataCellStyle="Output"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1001,174 +1073,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
+      <c r="C2" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7">
-        <f>Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
         <v>2</v>
       </c>
-      <c r="G2" s="7">
-        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[OpenMP_threads_per_rank]]</f>
+      <c r="I2" s="7">
+        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>2</v>
       </c>
-      <c r="H2" s="7">
-        <f>Table1[[#This Row],[OpenMP_threads_per_rank]]*Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
+      <c r="J2" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
         <v>2</v>
       </c>
-      <c r="I2" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[nodes]]</f>
+      <c r="K2" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>2</v>
       </c>
-      <c r="J2" s="10" t="b">
+      <c r="L2" s="10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6">
-        <v>1</v>
+      <c r="C3" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="D3" s="6">
         <v>1</v>
       </c>
       <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
         <v>2</v>
       </c>
-      <c r="F3" s="7">
-        <f>Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="G3" s="7">
-        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[OpenMP_threads_per_rank]]</f>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>2</v>
       </c>
-      <c r="H3" s="7">
-        <f>Table1[[#This Row],[OpenMP_threads_per_rank]]*Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
+      <c r="J3" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
         <v>2</v>
       </c>
-      <c r="I3" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[nodes]]</f>
+      <c r="K3" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>2</v>
       </c>
-      <c r="J3" s="7" t="b">
+      <c r="L3" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="6">
-        <v>1</v>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6">
         <v>2</v>
       </c>
-      <c r="F4" s="7">
-        <f>Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
+      <c r="F4" s="6">
         <v>2</v>
       </c>
-      <c r="G4" s="7">
-        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[OpenMP_threads_per_rank]]</f>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="7">
+        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[n_omp_threads]]</f>
         <v>4</v>
       </c>
-      <c r="H4" s="7">
-        <f>Table1[[#This Row],[OpenMP_threads_per_rank]]*Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
+      <c r="J4" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
         <v>4</v>
       </c>
-      <c r="I4" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[nodes]]</f>
+      <c r="K4" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
         <v>4</v>
       </c>
-      <c r="J4" s="7" t="b">
+      <c r="L4" s="7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
-        <v>1</v>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="6">
         <v>1</v>
@@ -1176,23 +1274,29 @@
       <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="7">
-        <f>Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="7">
-        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[OpenMP_threads_per_rank]]</f>
-        <v>1</v>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
       </c>
       <c r="H5" s="7">
-        <f>Table1[[#This Row],[OpenMP_threads_per_rank]]*Table1[[#This Row],[MPI_ranks_per_node]]*Table1[[#This Row],[nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="J5" s="7" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <f>Table1[[#This Row],[total_MPI_ranks]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+      <c r="K5" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+      <c r="L5" s="7" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>